<commit_message>
update test case excel
</commit_message>
<xml_diff>
--- a/test_case_excel/Test Case - LNK.xlsx
+++ b/test_case_excel/Test Case - LNK.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lnk-technical-test\test_case_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E013E452-F806-4749-B291-1E7CC0D45D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DB0B51-7F8C-41D3-8AAF-EDBDBA3F885B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
-    <sheet name="Tes Teori" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Feature</t>
   </si>
@@ -178,30 +177,6 @@
   <si>
     <t>User see alert/error messages that the question is required</t>
   </si>
-  <si>
-    <t>Verfikasi email dummy dapat menggunakan Mailslurp.</t>
-  </si>
-  <si>
-    <t>Langkah yg harus dilakukan adalah signup di website mailslurp.com</t>
-  </si>
-  <si>
-    <t>Setelah itu anda akan mendapatkan API key</t>
-  </si>
-  <si>
-    <t>API key di setting di dalam tools automation misal cypress</t>
-  </si>
-  <si>
-    <t>Petunjuknya bisa dilihat di link ini https://docs.mailslurp.com/cypress-mailslurp/</t>
-  </si>
-  <si>
-    <t>Setelah instalasi dan setup mailslurp-cypress selesai, maka anda dapat melakukan automation terhadap email dummy</t>
-  </si>
-  <si>
-    <t>Anda dapat mengirim ataupun menerima email dengan cara automation</t>
-  </si>
-  <si>
-    <t>Bahkan untuk testing terhadap OTP pun dapat dilakukan.</t>
-  </si>
 </sst>
 </file>
 
@@ -310,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -336,7 +311,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -636,10 +610,10 @@
       <c r="Y1" s="4"/>
     </row>
     <row r="2" spans="1:25" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -687,8 +661,8 @@
       <c r="Y2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
@@ -27620,60 +27594,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>